<commit_message>
Update WhatsApp message to simplified format: Quantity__
</commit_message>
<xml_diff>
--- a/data/master_df.xlsx
+++ b/data/master_df.xlsx
@@ -528,7 +528,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>1350</v>
+        <v>1250</v>
       </c>
       <c r="C6" t="inlineStr"/>
       <c r="D6" t="inlineStr"/>
@@ -542,7 +542,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>1225</v>
+        <v>1125</v>
       </c>
       <c r="C7" t="inlineStr"/>
       <c r="D7" t="inlineStr"/>
@@ -570,7 +570,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>2125</v>
+        <v>1875</v>
       </c>
       <c r="C9" t="inlineStr"/>
       <c r="D9" t="inlineStr"/>
@@ -584,7 +584,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>2825</v>
+        <v>4725</v>
       </c>
       <c r="C10" t="inlineStr"/>
       <c r="D10" t="inlineStr"/>
@@ -598,7 +598,7 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>10650</v>
+        <v>10250</v>
       </c>
       <c r="C11" t="inlineStr"/>
       <c r="D11" t="inlineStr"/>
@@ -654,7 +654,7 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>15050</v>
+        <v>14250</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
@@ -674,7 +674,7 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>12200</v>
+        <v>11850</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
@@ -782,7 +782,7 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>14100</v>
+        <v>14050</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
@@ -822,7 +822,7 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>2800</v>
+        <v>2600</v>
       </c>
       <c r="C23" t="inlineStr">
         <is>
@@ -842,7 +842,7 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>1900</v>
+        <v>950</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
@@ -876,7 +876,7 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>3600</v>
+        <v>2800</v>
       </c>
       <c r="C26" t="inlineStr">
         <is>
@@ -896,7 +896,7 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>2900</v>
+        <v>2800</v>
       </c>
       <c r="C27" t="inlineStr">
         <is>
@@ -916,7 +916,7 @@
         </is>
       </c>
       <c r="B28" t="n">
-        <v>4950</v>
+        <v>4850</v>
       </c>
       <c r="C28" t="inlineStr"/>
       <c r="D28" t="inlineStr"/>
@@ -948,7 +948,7 @@
         </is>
       </c>
       <c r="B30" t="n">
-        <v>2300</v>
+        <v>1900</v>
       </c>
       <c r="C30" t="inlineStr">
         <is>
@@ -972,7 +972,7 @@
         </is>
       </c>
       <c r="B31" t="n">
-        <v>8900</v>
+        <v>8550</v>
       </c>
       <c r="C31" t="inlineStr"/>
       <c r="D31" t="inlineStr"/>
@@ -1024,7 +1024,7 @@
         </is>
       </c>
       <c r="B34" t="n">
-        <v>17500</v>
+        <v>17400</v>
       </c>
       <c r="C34" t="inlineStr">
         <is>
@@ -1044,7 +1044,7 @@
         </is>
       </c>
       <c r="B35" t="n">
-        <v>17350</v>
+        <v>17200</v>
       </c>
       <c r="C35" t="inlineStr">
         <is>
@@ -1136,7 +1136,7 @@
         </is>
       </c>
       <c r="B40" t="n">
-        <v>3300</v>
+        <v>1300</v>
       </c>
       <c r="C40" t="inlineStr">
         <is>
@@ -1180,7 +1180,7 @@
         </is>
       </c>
       <c r="B42" t="n">
-        <v>1550</v>
+        <v>200</v>
       </c>
       <c r="C42" t="inlineStr">
         <is>
@@ -1200,7 +1200,7 @@
         </is>
       </c>
       <c r="B43" t="n">
-        <v>2800</v>
+        <v>2300</v>
       </c>
       <c r="C43" t="inlineStr">
         <is>
@@ -1446,7 +1446,7 @@
         </is>
       </c>
       <c r="B58" t="n">
-        <v>0</v>
+        <v>6875</v>
       </c>
       <c r="C58" t="inlineStr"/>
       <c r="D58" t="inlineStr"/>
@@ -1974,7 +1974,7 @@
         </is>
       </c>
       <c r="B89" t="n">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C89" t="inlineStr"/>
       <c r="D89" t="inlineStr"/>
@@ -1988,7 +1988,7 @@
         </is>
       </c>
       <c r="B90" t="n">
-        <v>-13</v>
+        <v>-18</v>
       </c>
       <c r="C90" t="inlineStr"/>
       <c r="D90" t="inlineStr"/>
@@ -2002,7 +2002,7 @@
         </is>
       </c>
       <c r="B91" t="n">
-        <v>-45</v>
+        <v>-57</v>
       </c>
       <c r="C91" t="inlineStr"/>
       <c r="D91" t="inlineStr"/>
@@ -2030,7 +2030,7 @@
         </is>
       </c>
       <c r="B93" t="n">
-        <v>-24</v>
+        <v>-34</v>
       </c>
       <c r="C93" t="inlineStr"/>
       <c r="D93" t="inlineStr"/>
@@ -2044,7 +2044,7 @@
         </is>
       </c>
       <c r="B94" t="n">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C94" t="inlineStr"/>
       <c r="D94" t="inlineStr"/>
@@ -2058,7 +2058,7 @@
         </is>
       </c>
       <c r="B95" t="n">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C95" t="inlineStr"/>
       <c r="D95" t="inlineStr"/>
@@ -2086,7 +2086,7 @@
         </is>
       </c>
       <c r="B97" t="n">
-        <v>-47</v>
+        <v>-49</v>
       </c>
       <c r="C97" t="inlineStr"/>
       <c r="D97" t="inlineStr"/>
@@ -2128,7 +2128,7 @@
         </is>
       </c>
       <c r="B100" t="n">
-        <v>-13</v>
+        <v>-27</v>
       </c>
       <c r="C100" t="inlineStr"/>
       <c r="D100" t="inlineStr"/>
@@ -2142,7 +2142,7 @@
         </is>
       </c>
       <c r="B101" t="n">
-        <v>2250</v>
+        <v>1750</v>
       </c>
       <c r="C101" t="inlineStr"/>
       <c r="D101" t="inlineStr"/>
@@ -2158,7 +2158,7 @@
         </is>
       </c>
       <c r="B102" t="n">
-        <v>3300</v>
+        <v>3150</v>
       </c>
       <c r="C102" t="inlineStr"/>
       <c r="D102" t="inlineStr"/>
@@ -2174,7 +2174,7 @@
         </is>
       </c>
       <c r="B103" t="n">
-        <v>1950</v>
+        <v>1550</v>
       </c>
       <c r="C103" t="inlineStr"/>
       <c r="D103" t="inlineStr"/>
@@ -2206,7 +2206,7 @@
         </is>
       </c>
       <c r="B105" t="n">
-        <v>2400</v>
+        <v>2300</v>
       </c>
       <c r="C105" t="inlineStr"/>
       <c r="D105" t="inlineStr"/>
@@ -2254,7 +2254,7 @@
         </is>
       </c>
       <c r="B108" t="n">
-        <v>2100</v>
+        <v>2000</v>
       </c>
       <c r="C108" t="inlineStr"/>
       <c r="D108" t="inlineStr"/>
@@ -2270,7 +2270,7 @@
         </is>
       </c>
       <c r="B109" t="n">
-        <v>2700</v>
+        <v>2300</v>
       </c>
       <c r="C109" t="inlineStr"/>
       <c r="D109" t="inlineStr"/>
@@ -2318,7 +2318,7 @@
         </is>
       </c>
       <c r="B112" t="n">
-        <v>650</v>
+        <v>300</v>
       </c>
       <c r="C112" t="inlineStr"/>
       <c r="D112" t="inlineStr"/>
@@ -2382,7 +2382,7 @@
         </is>
       </c>
       <c r="B116" t="n">
-        <v>350</v>
+        <v>1850</v>
       </c>
       <c r="C116" t="inlineStr"/>
       <c r="D116" t="inlineStr"/>
@@ -2398,7 +2398,7 @@
         </is>
       </c>
       <c r="B117" t="n">
-        <v>1100</v>
+        <v>1000</v>
       </c>
       <c r="C117" t="inlineStr"/>
       <c r="D117" t="inlineStr"/>
@@ -2446,7 +2446,7 @@
         </is>
       </c>
       <c r="B120" t="n">
-        <v>1100</v>
+        <v>1000</v>
       </c>
       <c r="C120" t="inlineStr"/>
       <c r="D120" t="inlineStr"/>
@@ -2462,7 +2462,7 @@
         </is>
       </c>
       <c r="B121" t="n">
-        <v>2450</v>
+        <v>2150</v>
       </c>
       <c r="C121" t="inlineStr"/>
       <c r="D121" t="inlineStr"/>
@@ -2478,7 +2478,7 @@
         </is>
       </c>
       <c r="B122" t="n">
-        <v>700</v>
+        <v>600</v>
       </c>
       <c r="C122" t="inlineStr"/>
       <c r="D122" t="inlineStr"/>
@@ -2526,7 +2526,7 @@
         </is>
       </c>
       <c r="B125" t="n">
-        <v>800</v>
+        <v>350</v>
       </c>
       <c r="C125" t="inlineStr"/>
       <c r="D125" t="inlineStr"/>
@@ -2542,7 +2542,7 @@
         </is>
       </c>
       <c r="B126" t="n">
-        <v>3050</v>
+        <v>1950</v>
       </c>
       <c r="C126" t="inlineStr"/>
       <c r="D126" t="inlineStr"/>
@@ -2574,7 +2574,7 @@
         </is>
       </c>
       <c r="B128" t="n">
-        <v>2150</v>
+        <v>2050</v>
       </c>
       <c r="C128" t="inlineStr"/>
       <c r="D128" t="inlineStr"/>
@@ -2638,7 +2638,7 @@
         </is>
       </c>
       <c r="B132" t="n">
-        <v>2400</v>
+        <v>2200</v>
       </c>
       <c r="C132" t="inlineStr"/>
       <c r="D132" t="inlineStr"/>
@@ -2654,7 +2654,7 @@
         </is>
       </c>
       <c r="B133" t="n">
-        <v>1800</v>
+        <v>1750</v>
       </c>
       <c r="C133" t="inlineStr"/>
       <c r="D133" t="inlineStr"/>
@@ -2670,7 +2670,7 @@
         </is>
       </c>
       <c r="B134" t="n">
-        <v>1600</v>
+        <v>1500</v>
       </c>
       <c r="C134" t="inlineStr"/>
       <c r="D134" t="inlineStr"/>
@@ -2772,7 +2772,7 @@
         </is>
       </c>
       <c r="B141" t="n">
-        <v>9400</v>
+        <v>8200</v>
       </c>
       <c r="C141" t="inlineStr"/>
       <c r="D141" t="inlineStr"/>
@@ -2816,7 +2816,7 @@
         </is>
       </c>
       <c r="B144" t="n">
-        <v>1500</v>
+        <v>1350</v>
       </c>
       <c r="C144" t="inlineStr">
         <is>
@@ -2864,7 +2864,7 @@
         </is>
       </c>
       <c r="B146" t="n">
-        <v>10900</v>
+        <v>10050</v>
       </c>
       <c r="C146" t="inlineStr">
         <is>
@@ -2900,7 +2900,7 @@
         </is>
       </c>
       <c r="B148" t="n">
-        <v>4482</v>
+        <v>4282</v>
       </c>
       <c r="C148" t="inlineStr"/>
       <c r="D148" t="inlineStr"/>
@@ -2932,7 +2932,7 @@
         </is>
       </c>
       <c r="B150" t="n">
-        <v>14200</v>
+        <v>13800</v>
       </c>
       <c r="C150" t="inlineStr"/>
       <c r="D150" t="inlineStr"/>
@@ -3036,7 +3036,7 @@
         </is>
       </c>
       <c r="B156" t="n">
-        <v>2750</v>
+        <v>2350</v>
       </c>
       <c r="C156" t="inlineStr"/>
       <c r="D156" t="inlineStr"/>
@@ -3132,7 +3132,7 @@
         </is>
       </c>
       <c r="B162" t="n">
-        <v>2050</v>
+        <v>1950</v>
       </c>
       <c r="C162" t="inlineStr"/>
       <c r="D162" t="inlineStr"/>
@@ -3148,7 +3148,7 @@
         </is>
       </c>
       <c r="B163" t="n">
-        <v>1800</v>
+        <v>1700</v>
       </c>
       <c r="C163" t="inlineStr">
         <is>
@@ -3200,7 +3200,7 @@
         </is>
       </c>
       <c r="B166" t="n">
-        <v>3850</v>
+        <v>3350</v>
       </c>
       <c r="C166" t="inlineStr">
         <is>
@@ -3236,7 +3236,7 @@
         </is>
       </c>
       <c r="B168" t="n">
-        <v>5150</v>
+        <v>4100</v>
       </c>
       <c r="C168" t="inlineStr">
         <is>
@@ -3256,7 +3256,7 @@
         </is>
       </c>
       <c r="B169" t="n">
-        <v>1300</v>
+        <v>1200</v>
       </c>
       <c r="C169" t="inlineStr"/>
       <c r="D169" t="inlineStr"/>
@@ -3324,7 +3324,7 @@
         </is>
       </c>
       <c r="B173" t="n">
-        <v>7150</v>
+        <v>6650</v>
       </c>
       <c r="C173" t="inlineStr"/>
       <c r="D173" t="inlineStr"/>
@@ -3340,7 +3340,7 @@
         </is>
       </c>
       <c r="B174" t="n">
-        <v>9900</v>
+        <v>9600</v>
       </c>
       <c r="C174" t="inlineStr">
         <is>
@@ -3360,7 +3360,7 @@
         </is>
       </c>
       <c r="B175" t="n">
-        <v>7700</v>
+        <v>7600</v>
       </c>
       <c r="C175" t="inlineStr">
         <is>
@@ -3400,7 +3400,7 @@
         </is>
       </c>
       <c r="B177" t="n">
-        <v>300</v>
+        <v>0</v>
       </c>
       <c r="C177" t="inlineStr">
         <is>
@@ -3420,7 +3420,7 @@
         </is>
       </c>
       <c r="B178" t="n">
-        <v>6800</v>
+        <v>6650</v>
       </c>
       <c r="C178" t="inlineStr"/>
       <c r="D178" t="inlineStr"/>
@@ -3452,7 +3452,7 @@
         </is>
       </c>
       <c r="B180" t="n">
-        <v>8550</v>
+        <v>7750</v>
       </c>
       <c r="C180" t="inlineStr">
         <is>
@@ -3472,7 +3472,7 @@
         </is>
       </c>
       <c r="B181" t="n">
-        <v>3700</v>
+        <v>2900</v>
       </c>
       <c r="C181" t="inlineStr">
         <is>
@@ -3492,7 +3492,7 @@
         </is>
       </c>
       <c r="B182" t="n">
-        <v>2600</v>
+        <v>1250</v>
       </c>
       <c r="C182" t="inlineStr">
         <is>
@@ -3512,7 +3512,7 @@
         </is>
       </c>
       <c r="B183" t="n">
-        <v>3300</v>
+        <v>2200</v>
       </c>
       <c r="C183" t="inlineStr">
         <is>
@@ -3532,7 +3532,7 @@
         </is>
       </c>
       <c r="B184" t="n">
-        <v>3650</v>
+        <v>2950</v>
       </c>
       <c r="C184" t="inlineStr"/>
       <c r="D184" t="inlineStr"/>
@@ -3548,7 +3548,7 @@
         </is>
       </c>
       <c r="B185" t="n">
-        <v>4400</v>
+        <v>4300</v>
       </c>
       <c r="C185" t="inlineStr">
         <is>
@@ -3568,7 +3568,7 @@
         </is>
       </c>
       <c r="B186" t="n">
-        <v>5800</v>
+        <v>5550</v>
       </c>
       <c r="C186" t="inlineStr">
         <is>
@@ -3608,7 +3608,7 @@
         </is>
       </c>
       <c r="B188" t="n">
-        <v>6100</v>
+        <v>4800</v>
       </c>
       <c r="C188" t="inlineStr">
         <is>
@@ -3628,7 +3628,7 @@
         </is>
       </c>
       <c r="B189" t="n">
-        <v>300</v>
+        <v>50</v>
       </c>
       <c r="C189" t="inlineStr">
         <is>
@@ -3648,7 +3648,7 @@
         </is>
       </c>
       <c r="B190" t="n">
-        <v>400</v>
+        <v>-100</v>
       </c>
       <c r="C190" t="inlineStr">
         <is>
@@ -3676,7 +3676,7 @@
         </is>
       </c>
       <c r="B191" t="n">
-        <v>3850</v>
+        <v>3550</v>
       </c>
       <c r="C191" t="inlineStr"/>
       <c r="D191" t="inlineStr"/>
@@ -3692,7 +3692,7 @@
         </is>
       </c>
       <c r="B192" t="n">
-        <v>2700</v>
+        <v>2150</v>
       </c>
       <c r="C192" t="inlineStr">
         <is>
@@ -3736,7 +3736,7 @@
         </is>
       </c>
       <c r="B194" t="n">
-        <v>3700</v>
+        <v>3200</v>
       </c>
       <c r="C194" t="inlineStr">
         <is>
@@ -3764,7 +3764,7 @@
         </is>
       </c>
       <c r="B195" t="n">
-        <v>9800</v>
+        <v>9300</v>
       </c>
       <c r="C195" t="inlineStr">
         <is>
@@ -3792,7 +3792,7 @@
         </is>
       </c>
       <c r="B196" t="n">
-        <v>1500</v>
+        <v>6400</v>
       </c>
       <c r="C196" t="inlineStr">
         <is>
@@ -3836,7 +3836,7 @@
         </is>
       </c>
       <c r="B198" t="n">
-        <v>2600</v>
+        <v>2100</v>
       </c>
       <c r="C198" t="inlineStr">
         <is>
@@ -3900,7 +3900,7 @@
         </is>
       </c>
       <c r="B201" t="n">
-        <v>3500</v>
+        <v>12800</v>
       </c>
       <c r="C201" t="inlineStr">
         <is>
@@ -3924,7 +3924,7 @@
         </is>
       </c>
       <c r="B202" t="n">
-        <v>1900</v>
+        <v>5200</v>
       </c>
       <c r="C202" t="inlineStr">
         <is>
@@ -4004,7 +4004,7 @@
         </is>
       </c>
       <c r="B207" t="n">
-        <v>1350</v>
+        <v>900</v>
       </c>
       <c r="C207" t="inlineStr"/>
       <c r="D207" t="inlineStr"/>
@@ -4052,7 +4052,7 @@
         </is>
       </c>
       <c r="B210" t="n">
-        <v>3050</v>
+        <v>750</v>
       </c>
       <c r="C210" t="inlineStr">
         <is>
@@ -4076,7 +4076,7 @@
         </is>
       </c>
       <c r="B211" t="n">
-        <v>13600</v>
+        <v>13200</v>
       </c>
       <c r="C211" t="inlineStr">
         <is>
@@ -4112,7 +4112,7 @@
         </is>
       </c>
       <c r="B213" t="n">
-        <v>4200</v>
+        <v>3600</v>
       </c>
       <c r="C213" t="inlineStr">
         <is>
@@ -4132,7 +4132,7 @@
         </is>
       </c>
       <c r="B214" t="n">
-        <v>7350</v>
+        <v>1200</v>
       </c>
       <c r="C214" t="inlineStr">
         <is>
@@ -4152,7 +4152,7 @@
         </is>
       </c>
       <c r="B215" t="n">
-        <v>3600</v>
+        <v>2000</v>
       </c>
       <c r="C215" t="inlineStr">
         <is>
@@ -4220,7 +4220,7 @@
         </is>
       </c>
       <c r="B219" t="n">
-        <v>4900</v>
+        <v>4700</v>
       </c>
       <c r="C219" t="inlineStr">
         <is>
@@ -4264,7 +4264,7 @@
         </is>
       </c>
       <c r="B221" t="n">
-        <v>1350</v>
+        <v>700</v>
       </c>
       <c r="C221" t="inlineStr">
         <is>
@@ -4284,7 +4284,7 @@
         </is>
       </c>
       <c r="B222" t="n">
-        <v>3000</v>
+        <v>2600</v>
       </c>
       <c r="C222" t="inlineStr"/>
       <c r="D222" t="inlineStr"/>
@@ -4384,7 +4384,7 @@
         </is>
       </c>
       <c r="B228" t="n">
-        <v>1900</v>
+        <v>5100</v>
       </c>
       <c r="C228" t="inlineStr">
         <is>
@@ -4408,7 +4408,7 @@
         </is>
       </c>
       <c r="B229" t="n">
-        <v>5550</v>
+        <v>3950</v>
       </c>
       <c r="C229" t="inlineStr">
         <is>
@@ -4480,7 +4480,7 @@
         </is>
       </c>
       <c r="B233" t="n">
-        <v>2000</v>
+        <v>500</v>
       </c>
       <c r="C233" t="inlineStr">
         <is>
@@ -4540,7 +4540,7 @@
         </is>
       </c>
       <c r="B236" t="n">
-        <v>2000</v>
+        <v>1900</v>
       </c>
       <c r="C236" t="inlineStr">
         <is>
@@ -4560,7 +4560,7 @@
         </is>
       </c>
       <c r="B237" t="n">
-        <v>3100</v>
+        <v>4400</v>
       </c>
       <c r="C237" t="inlineStr">
         <is>
@@ -4580,7 +4580,7 @@
         </is>
       </c>
       <c r="B238" t="n">
-        <v>1300</v>
+        <v>3300</v>
       </c>
       <c r="C238" t="inlineStr"/>
       <c r="D238" t="inlineStr"/>
@@ -4596,7 +4596,7 @@
         </is>
       </c>
       <c r="B239" t="n">
-        <v>7100</v>
+        <v>6200</v>
       </c>
       <c r="C239" t="inlineStr"/>
       <c r="D239" t="inlineStr"/>
@@ -4612,7 +4612,7 @@
         </is>
       </c>
       <c r="B240" t="n">
-        <v>5250</v>
+        <v>4950</v>
       </c>
       <c r="C240" t="inlineStr"/>
       <c r="D240" t="inlineStr"/>
@@ -4644,7 +4644,7 @@
         </is>
       </c>
       <c r="B242" t="n">
-        <v>1450</v>
+        <v>1300</v>
       </c>
       <c r="C242" t="inlineStr"/>
       <c r="D242" t="inlineStr"/>
@@ -4704,7 +4704,7 @@
         </is>
       </c>
       <c r="B245" t="n">
-        <v>2400</v>
+        <v>2050</v>
       </c>
       <c r="C245" t="inlineStr">
         <is>
@@ -4740,7 +4740,7 @@
         </is>
       </c>
       <c r="B247" t="n">
-        <v>7550</v>
+        <v>7400</v>
       </c>
       <c r="C247" t="inlineStr"/>
       <c r="D247" t="inlineStr"/>
@@ -4756,7 +4756,7 @@
         </is>
       </c>
       <c r="B248" t="n">
-        <v>450</v>
+        <v>-50</v>
       </c>
       <c r="C248" t="inlineStr">
         <is>
@@ -4780,7 +4780,7 @@
         </is>
       </c>
       <c r="B249" t="n">
-        <v>2150</v>
+        <v>1650</v>
       </c>
       <c r="C249" t="inlineStr">
         <is>
@@ -4820,7 +4820,7 @@
         </is>
       </c>
       <c r="B251" t="n">
-        <v>5600</v>
+        <v>5450</v>
       </c>
       <c r="C251" t="inlineStr">
         <is>
@@ -4840,7 +4840,7 @@
         </is>
       </c>
       <c r="B252" t="n">
-        <v>3300</v>
+        <v>2800</v>
       </c>
       <c r="C252" t="inlineStr">
         <is>
@@ -4916,7 +4916,7 @@
         </is>
       </c>
       <c r="B256" t="n">
-        <v>6400</v>
+        <v>6650</v>
       </c>
       <c r="C256" t="inlineStr">
         <is>
@@ -4960,7 +4960,7 @@
         </is>
       </c>
       <c r="B258" t="n">
-        <v>6200</v>
+        <v>5600</v>
       </c>
       <c r="C258" t="inlineStr">
         <is>
@@ -4996,7 +4996,7 @@
         </is>
       </c>
       <c r="B260" t="n">
-        <v>1950</v>
+        <v>1850</v>
       </c>
       <c r="C260" t="inlineStr"/>
       <c r="D260" t="inlineStr"/>
@@ -5012,7 +5012,7 @@
         </is>
       </c>
       <c r="B261" t="n">
-        <v>350</v>
+        <v>1700</v>
       </c>
       <c r="C261" t="inlineStr">
         <is>
@@ -5036,7 +5036,7 @@
         </is>
       </c>
       <c r="B262" t="n">
-        <v>3300</v>
+        <v>2700</v>
       </c>
       <c r="C262" t="inlineStr">
         <is>
@@ -5056,7 +5056,7 @@
         </is>
       </c>
       <c r="B263" t="n">
-        <v>7550</v>
+        <v>7050</v>
       </c>
       <c r="C263" t="inlineStr">
         <is>
@@ -5076,7 +5076,7 @@
         </is>
       </c>
       <c r="B264" t="n">
-        <v>2750</v>
+        <v>2650</v>
       </c>
       <c r="C264" t="inlineStr"/>
       <c r="D264" t="inlineStr"/>
@@ -5092,7 +5092,7 @@
         </is>
       </c>
       <c r="B265" t="n">
-        <v>1750</v>
+        <v>1850</v>
       </c>
       <c r="C265" t="inlineStr"/>
       <c r="D265" t="inlineStr"/>
@@ -5124,7 +5124,7 @@
         </is>
       </c>
       <c r="B267" t="n">
-        <v>17500</v>
+        <v>16500</v>
       </c>
       <c r="C267" t="inlineStr">
         <is>
@@ -5144,7 +5144,7 @@
         </is>
       </c>
       <c r="B268" t="n">
-        <v>1300</v>
+        <v>1700</v>
       </c>
       <c r="C268" t="inlineStr">
         <is>
@@ -5314,7 +5314,7 @@
         </is>
       </c>
       <c r="B278" t="n">
-        <v>1485</v>
+        <v>1035</v>
       </c>
       <c r="C278" t="inlineStr"/>
       <c r="D278" t="inlineStr"/>
@@ -5410,7 +5410,7 @@
         </is>
       </c>
       <c r="B284" t="n">
-        <v>850</v>
+        <v>750</v>
       </c>
       <c r="C284" t="inlineStr"/>
       <c r="D284" t="inlineStr"/>
@@ -5466,7 +5466,7 @@
         </is>
       </c>
       <c r="B287" t="n">
-        <v>3400</v>
+        <v>3150</v>
       </c>
       <c r="C287" t="inlineStr"/>
       <c r="D287" t="inlineStr"/>
@@ -5498,7 +5498,7 @@
         </is>
       </c>
       <c r="B289" t="n">
-        <v>1200</v>
+        <v>1000</v>
       </c>
       <c r="C289" t="inlineStr"/>
       <c r="D289" t="inlineStr"/>
@@ -5530,7 +5530,7 @@
         </is>
       </c>
       <c r="B291" t="n">
-        <v>1600</v>
+        <v>1450</v>
       </c>
       <c r="C291" t="inlineStr"/>
       <c r="D291" t="inlineStr"/>
@@ -5578,7 +5578,7 @@
         </is>
       </c>
       <c r="B294" t="n">
-        <v>6700</v>
+        <v>6000</v>
       </c>
       <c r="C294" t="inlineStr">
         <is>
@@ -5598,7 +5598,7 @@
         </is>
       </c>
       <c r="B295" t="n">
-        <v>3100</v>
+        <v>2700</v>
       </c>
       <c r="C295" t="inlineStr">
         <is>
@@ -5634,7 +5634,7 @@
         </is>
       </c>
       <c r="B297" t="n">
-        <v>1550</v>
+        <v>2450</v>
       </c>
       <c r="C297" t="inlineStr">
         <is>
@@ -5688,7 +5688,7 @@
         </is>
       </c>
       <c r="B300" t="n">
-        <v>3550</v>
+        <v>1750</v>
       </c>
       <c r="C300" t="inlineStr">
         <is>
@@ -5732,7 +5732,7 @@
         </is>
       </c>
       <c r="B302" t="n">
-        <v>2950</v>
+        <v>1100</v>
       </c>
       <c r="C302" t="inlineStr">
         <is>
@@ -5776,7 +5776,7 @@
         </is>
       </c>
       <c r="B304" t="n">
-        <v>2900</v>
+        <v>1950</v>
       </c>
       <c r="C304" t="inlineStr">
         <is>
@@ -5800,7 +5800,7 @@
         </is>
       </c>
       <c r="B305" t="n">
-        <v>1450</v>
+        <v>1050</v>
       </c>
       <c r="C305" t="inlineStr">
         <is>
@@ -5864,7 +5864,7 @@
         </is>
       </c>
       <c r="B308" t="n">
-        <v>5950</v>
+        <v>5900</v>
       </c>
       <c r="C308" t="inlineStr"/>
       <c r="D308" t="inlineStr"/>
@@ -5948,7 +5948,7 @@
         </is>
       </c>
       <c r="B313" t="n">
-        <v>3300</v>
+        <v>2600</v>
       </c>
       <c r="C313" t="inlineStr">
         <is>
@@ -5968,7 +5968,7 @@
         </is>
       </c>
       <c r="B314" t="n">
-        <v>4950</v>
+        <v>3750</v>
       </c>
       <c r="C314" t="inlineStr">
         <is>
@@ -6008,7 +6008,7 @@
         </is>
       </c>
       <c r="B316" t="n">
-        <v>2550</v>
+        <v>1750</v>
       </c>
       <c r="C316" t="inlineStr">
         <is>
@@ -6032,7 +6032,7 @@
         </is>
       </c>
       <c r="B317" t="n">
-        <v>-200</v>
+        <v>1000</v>
       </c>
       <c r="C317" t="inlineStr">
         <is>
@@ -6052,7 +6052,7 @@
         </is>
       </c>
       <c r="B318" t="n">
-        <v>2100</v>
+        <v>2900</v>
       </c>
       <c r="C318" t="inlineStr"/>
       <c r="D318" t="inlineStr"/>
@@ -6100,7 +6100,7 @@
         </is>
       </c>
       <c r="B321" t="n">
-        <v>2100</v>
+        <v>1100</v>
       </c>
       <c r="C321" t="inlineStr"/>
       <c r="D321" t="inlineStr"/>
@@ -6172,7 +6172,7 @@
         </is>
       </c>
       <c r="B325" t="n">
-        <v>1450</v>
+        <v>-700</v>
       </c>
       <c r="C325" t="inlineStr">
         <is>
@@ -6236,7 +6236,7 @@
         </is>
       </c>
       <c r="B328" t="n">
-        <v>1950</v>
+        <v>1150</v>
       </c>
       <c r="C328" t="inlineStr">
         <is>
@@ -6260,7 +6260,7 @@
         </is>
       </c>
       <c r="B329" t="n">
-        <v>700</v>
+        <v>0</v>
       </c>
       <c r="C329" t="inlineStr"/>
       <c r="D329" t="inlineStr"/>
@@ -6292,7 +6292,7 @@
         </is>
       </c>
       <c r="B331" t="n">
-        <v>-300</v>
+        <v>650</v>
       </c>
       <c r="C331" t="inlineStr">
         <is>
@@ -6332,7 +6332,7 @@
         </is>
       </c>
       <c r="B333" t="n">
-        <v>0</v>
+        <v>-1000</v>
       </c>
       <c r="C333" t="inlineStr"/>
       <c r="D333" t="inlineStr"/>
@@ -6348,7 +6348,7 @@
         </is>
       </c>
       <c r="B334" t="n">
-        <v>2500</v>
+        <v>1900</v>
       </c>
       <c r="C334" t="inlineStr">
         <is>
@@ -6384,7 +6384,7 @@
         </is>
       </c>
       <c r="B336" t="n">
-        <v>3400</v>
+        <v>2900</v>
       </c>
       <c r="C336" t="inlineStr"/>
       <c r="D336" t="inlineStr"/>
@@ -6400,7 +6400,7 @@
         </is>
       </c>
       <c r="B337" t="n">
-        <v>1250</v>
+        <v>850</v>
       </c>
       <c r="C337" t="inlineStr">
         <is>
@@ -6424,7 +6424,7 @@
         </is>
       </c>
       <c r="B338" t="n">
-        <v>4350</v>
+        <v>2050</v>
       </c>
       <c r="C338" t="inlineStr">
         <is>
@@ -6444,7 +6444,7 @@
         </is>
       </c>
       <c r="B339" t="n">
-        <v>2250</v>
+        <v>2200</v>
       </c>
       <c r="C339" t="inlineStr"/>
       <c r="D339" t="inlineStr"/>
@@ -6480,7 +6480,7 @@
         </is>
       </c>
       <c r="B341" t="n">
-        <v>1500</v>
+        <v>1350</v>
       </c>
       <c r="C341" t="inlineStr">
         <is>
@@ -6520,7 +6520,7 @@
         </is>
       </c>
       <c r="B343" t="n">
-        <v>2000</v>
+        <v>1400</v>
       </c>
       <c r="C343" t="inlineStr"/>
       <c r="D343" t="inlineStr"/>
@@ -6536,7 +6536,7 @@
         </is>
       </c>
       <c r="B344" t="n">
-        <v>4100</v>
+        <v>3600</v>
       </c>
       <c r="C344" t="inlineStr">
         <is>
@@ -6556,7 +6556,7 @@
         </is>
       </c>
       <c r="B345" t="n">
-        <v>6500</v>
+        <v>6300</v>
       </c>
       <c r="C345" t="inlineStr">
         <is>
@@ -6576,7 +6576,7 @@
         </is>
       </c>
       <c r="B346" t="n">
-        <v>1500</v>
+        <v>1300</v>
       </c>
       <c r="C346" t="inlineStr">
         <is>
@@ -6736,7 +6736,7 @@
         </is>
       </c>
       <c r="B355" t="n">
-        <v>300</v>
+        <v>0</v>
       </c>
       <c r="C355" t="inlineStr"/>
       <c r="D355" t="inlineStr"/>
@@ -6752,7 +6752,7 @@
         </is>
       </c>
       <c r="B356" t="n">
-        <v>1650</v>
+        <v>1200</v>
       </c>
       <c r="C356" t="inlineStr"/>
       <c r="D356" t="inlineStr"/>
@@ -6812,7 +6812,7 @@
         </is>
       </c>
       <c r="B359" t="n">
-        <v>350</v>
+        <v>200</v>
       </c>
       <c r="C359" t="inlineStr"/>
       <c r="D359" t="inlineStr"/>
@@ -6848,7 +6848,7 @@
         </is>
       </c>
       <c r="B361" t="n">
-        <v>800</v>
+        <v>700</v>
       </c>
       <c r="C361" t="inlineStr">
         <is>
@@ -6884,7 +6884,7 @@
         </is>
       </c>
       <c r="B363" t="n">
-        <v>2450</v>
+        <v>2200</v>
       </c>
       <c r="C363" t="inlineStr">
         <is>
@@ -6944,7 +6944,7 @@
         </is>
       </c>
       <c r="B366" t="n">
-        <v>1850</v>
+        <v>950</v>
       </c>
       <c r="C366" t="inlineStr">
         <is>
@@ -6968,7 +6968,7 @@
         </is>
       </c>
       <c r="B367" t="n">
-        <v>4250</v>
+        <v>2250</v>
       </c>
       <c r="C367" t="inlineStr">
         <is>
@@ -7056,7 +7056,7 @@
         </is>
       </c>
       <c r="B372" t="n">
-        <v>1800</v>
+        <v>1400</v>
       </c>
       <c r="C372" t="inlineStr">
         <is>
@@ -7092,7 +7092,7 @@
         </is>
       </c>
       <c r="B374" t="n">
-        <v>1600</v>
+        <v>800</v>
       </c>
       <c r="C374" t="inlineStr"/>
       <c r="D374" t="inlineStr"/>
@@ -7124,7 +7124,7 @@
         </is>
       </c>
       <c r="B376" t="n">
-        <v>50</v>
+        <v>-950</v>
       </c>
       <c r="C376" t="inlineStr"/>
       <c r="D376" t="inlineStr"/>
@@ -7180,7 +7180,7 @@
         </is>
       </c>
       <c r="B379" t="n">
-        <v>6250</v>
+        <v>6000</v>
       </c>
       <c r="C379" t="inlineStr">
         <is>
@@ -7216,7 +7216,7 @@
         </is>
       </c>
       <c r="B381" t="n">
-        <v>3450</v>
+        <v>3250</v>
       </c>
       <c r="C381" t="inlineStr">
         <is>
@@ -7252,7 +7252,7 @@
         </is>
       </c>
       <c r="B383" t="n">
-        <v>950</v>
+        <v>850</v>
       </c>
       <c r="C383" t="inlineStr"/>
       <c r="D383" t="inlineStr"/>
@@ -7268,7 +7268,7 @@
         </is>
       </c>
       <c r="B384" t="n">
-        <v>1800</v>
+        <v>1650</v>
       </c>
       <c r="C384" t="inlineStr">
         <is>
@@ -7288,7 +7288,7 @@
         </is>
       </c>
       <c r="B385" t="n">
-        <v>1500</v>
+        <v>1350</v>
       </c>
       <c r="C385" t="inlineStr"/>
       <c r="D385" t="inlineStr"/>
@@ -7420,7 +7420,7 @@
         </is>
       </c>
       <c r="B393" t="n">
-        <v>900</v>
+        <v>1400</v>
       </c>
       <c r="C393" t="inlineStr"/>
       <c r="D393" t="inlineStr"/>
@@ -7514,7 +7514,7 @@
         </is>
       </c>
       <c r="B399" t="n">
-        <v>450</v>
+        <v>2450</v>
       </c>
       <c r="C399" t="inlineStr"/>
       <c r="D399" t="inlineStr"/>
@@ -7530,7 +7530,7 @@
         </is>
       </c>
       <c r="B400" t="n">
-        <v>700</v>
+        <v>300</v>
       </c>
       <c r="C400" t="inlineStr"/>
       <c r="D400" t="inlineStr"/>
@@ -7546,7 +7546,7 @@
         </is>
       </c>
       <c r="B401" t="n">
-        <v>800</v>
+        <v>600</v>
       </c>
       <c r="C401" t="inlineStr"/>
       <c r="D401" t="inlineStr"/>
@@ -7594,7 +7594,7 @@
         </is>
       </c>
       <c r="B404" t="n">
-        <v>950</v>
+        <v>650</v>
       </c>
       <c r="C404" t="inlineStr"/>
       <c r="D404" t="inlineStr"/>
@@ -7752,7 +7752,7 @@
         </is>
       </c>
       <c r="B414" t="n">
-        <v>850</v>
+        <v>550</v>
       </c>
       <c r="C414" t="inlineStr"/>
       <c r="D414" t="inlineStr"/>
@@ -7768,7 +7768,7 @@
         </is>
       </c>
       <c r="B415" t="n">
-        <v>850</v>
+        <v>950</v>
       </c>
       <c r="C415" t="inlineStr"/>
       <c r="D415" t="inlineStr"/>
@@ -7816,7 +7816,7 @@
         </is>
       </c>
       <c r="B418" t="n">
-        <v>1000</v>
+        <v>1600</v>
       </c>
       <c r="C418" t="inlineStr"/>
       <c r="D418" t="inlineStr"/>
@@ -7848,7 +7848,7 @@
         </is>
       </c>
       <c r="B420" t="n">
-        <v>1750</v>
+        <v>1500</v>
       </c>
       <c r="C420" t="inlineStr"/>
       <c r="D420" t="inlineStr"/>
@@ -7896,7 +7896,7 @@
         </is>
       </c>
       <c r="B423" t="n">
-        <v>150</v>
+        <v>-250</v>
       </c>
       <c r="C423" t="inlineStr"/>
       <c r="D423" t="inlineStr"/>
@@ -7912,7 +7912,7 @@
         </is>
       </c>
       <c r="B424" t="n">
-        <v>4566</v>
+        <v>4316</v>
       </c>
       <c r="C424" t="inlineStr"/>
       <c r="D424" t="inlineStr"/>
@@ -8020,7 +8020,7 @@
         </is>
       </c>
       <c r="B431" t="n">
-        <v>1050</v>
+        <v>150</v>
       </c>
       <c r="C431" t="inlineStr"/>
       <c r="D431" t="inlineStr"/>
@@ -8052,7 +8052,7 @@
         </is>
       </c>
       <c r="B433" t="n">
-        <v>2700</v>
+        <v>1250</v>
       </c>
       <c r="C433" t="inlineStr"/>
       <c r="D433" t="inlineStr"/>
@@ -8068,7 +8068,7 @@
         </is>
       </c>
       <c r="B434" t="n">
-        <v>1425</v>
+        <v>1325</v>
       </c>
       <c r="C434" t="inlineStr"/>
       <c r="D434" t="inlineStr"/>
@@ -8100,7 +8100,7 @@
         </is>
       </c>
       <c r="B436" t="n">
-        <v>2200</v>
+        <v>1850</v>
       </c>
       <c r="C436" t="inlineStr"/>
       <c r="D436" t="inlineStr"/>
@@ -8116,7 +8116,7 @@
         </is>
       </c>
       <c r="B437" t="n">
-        <v>1500</v>
+        <v>1050</v>
       </c>
       <c r="C437" t="inlineStr"/>
       <c r="D437" t="inlineStr"/>
@@ -8274,7 +8274,7 @@
         </is>
       </c>
       <c r="B447" t="n">
-        <v>650</v>
+        <v>250</v>
       </c>
       <c r="C447" t="inlineStr"/>
       <c r="D447" t="inlineStr"/>
@@ -8290,7 +8290,7 @@
         </is>
       </c>
       <c r="B448" t="n">
-        <v>550</v>
+        <v>1150</v>
       </c>
       <c r="C448" t="inlineStr"/>
       <c r="D448" t="inlineStr"/>
@@ -8322,7 +8322,7 @@
         </is>
       </c>
       <c r="B450" t="n">
-        <v>1850</v>
+        <v>1750</v>
       </c>
       <c r="C450" t="inlineStr"/>
       <c r="D450" t="inlineStr"/>
@@ -8370,7 +8370,7 @@
         </is>
       </c>
       <c r="B453" t="n">
-        <v>2700</v>
+        <v>1350</v>
       </c>
       <c r="C453" t="inlineStr"/>
       <c r="D453" t="inlineStr"/>
@@ -8416,7 +8416,7 @@
         </is>
       </c>
       <c r="B456" t="n">
-        <v>1050</v>
+        <v>450</v>
       </c>
       <c r="C456" t="inlineStr"/>
       <c r="D456" t="inlineStr"/>
@@ -8464,7 +8464,7 @@
         </is>
       </c>
       <c r="B459" t="n">
-        <v>-600</v>
+        <v>-750</v>
       </c>
       <c r="C459" t="inlineStr"/>
       <c r="D459" t="inlineStr"/>
@@ -8512,7 +8512,7 @@
         </is>
       </c>
       <c r="B462" t="n">
-        <v>900</v>
+        <v>800</v>
       </c>
       <c r="C462" t="inlineStr"/>
       <c r="D462" t="inlineStr"/>
@@ -8572,7 +8572,7 @@
         </is>
       </c>
       <c r="B466" t="n">
-        <v>2100</v>
+        <v>1900</v>
       </c>
       <c r="C466" t="inlineStr"/>
       <c r="D466" t="inlineStr"/>
@@ -8588,7 +8588,7 @@
         </is>
       </c>
       <c r="B467" t="n">
-        <v>600</v>
+        <v>1300</v>
       </c>
       <c r="C467" t="inlineStr"/>
       <c r="D467" t="inlineStr"/>
@@ -8692,7 +8692,7 @@
         </is>
       </c>
       <c r="B474" t="n">
-        <v>2730</v>
+        <v>2630</v>
       </c>
       <c r="C474" t="inlineStr"/>
       <c r="D474" t="inlineStr"/>
@@ -8786,7 +8786,7 @@
         </is>
       </c>
       <c r="B480" t="n">
-        <v>1600</v>
+        <v>1500</v>
       </c>
       <c r="C480" t="inlineStr"/>
       <c r="D480" t="inlineStr"/>
@@ -8834,7 +8834,7 @@
         </is>
       </c>
       <c r="B483" t="n">
-        <v>19100</v>
+        <v>18300</v>
       </c>
       <c r="C483" t="inlineStr"/>
       <c r="D483" t="inlineStr"/>
@@ -8882,7 +8882,7 @@
         </is>
       </c>
       <c r="B486" t="n">
-        <v>7500</v>
+        <v>7000</v>
       </c>
       <c r="C486" t="inlineStr"/>
       <c r="D486" t="inlineStr"/>
@@ -8898,7 +8898,7 @@
         </is>
       </c>
       <c r="B487" t="n">
-        <v>7600</v>
+        <v>6600</v>
       </c>
       <c r="C487" t="inlineStr"/>
       <c r="D487" t="inlineStr"/>
@@ -8914,7 +8914,7 @@
         </is>
       </c>
       <c r="B488" t="n">
-        <v>9350</v>
+        <v>9250</v>
       </c>
       <c r="C488" t="inlineStr"/>
       <c r="D488" t="inlineStr"/>
@@ -8930,7 +8930,7 @@
         </is>
       </c>
       <c r="B489" t="n">
-        <v>6300</v>
+        <v>6150</v>
       </c>
       <c r="C489" t="inlineStr"/>
       <c r="D489" t="inlineStr"/>
@@ -8946,7 +8946,7 @@
         </is>
       </c>
       <c r="B490" t="n">
-        <v>4500</v>
+        <v>3600</v>
       </c>
       <c r="C490" t="inlineStr"/>
       <c r="D490" t="inlineStr"/>
@@ -9056,7 +9056,7 @@
         </is>
       </c>
       <c r="B497" t="n">
-        <v>3650</v>
+        <v>3550</v>
       </c>
       <c r="C497" t="inlineStr"/>
       <c r="D497" t="inlineStr"/>
@@ -9072,7 +9072,7 @@
         </is>
       </c>
       <c r="B498" t="n">
-        <v>2950</v>
+        <v>2250</v>
       </c>
       <c r="C498" t="inlineStr"/>
       <c r="D498" t="inlineStr"/>
@@ -9088,7 +9088,7 @@
         </is>
       </c>
       <c r="B499" t="n">
-        <v>2200</v>
+        <v>4600</v>
       </c>
       <c r="C499" t="inlineStr"/>
       <c r="D499" t="inlineStr"/>
@@ -9104,7 +9104,7 @@
         </is>
       </c>
       <c r="B500" t="n">
-        <v>150</v>
+        <v>-150</v>
       </c>
       <c r="C500" t="inlineStr"/>
       <c r="D500" t="inlineStr"/>
@@ -9136,7 +9136,7 @@
         </is>
       </c>
       <c r="B502" t="n">
-        <v>2300</v>
+        <v>1950</v>
       </c>
       <c r="C502" t="inlineStr">
         <is>
@@ -9172,7 +9172,7 @@
         </is>
       </c>
       <c r="B504" t="n">
-        <v>800</v>
+        <v>0</v>
       </c>
       <c r="C504" t="inlineStr"/>
       <c r="D504" t="inlineStr"/>
@@ -9188,7 +9188,7 @@
         </is>
       </c>
       <c r="B505" t="n">
-        <v>7000</v>
+        <v>6800</v>
       </c>
       <c r="C505" t="inlineStr"/>
       <c r="D505" t="inlineStr"/>
@@ -9204,7 +9204,7 @@
         </is>
       </c>
       <c r="B506" t="n">
-        <v>1300</v>
+        <v>300</v>
       </c>
       <c r="C506" t="inlineStr"/>
       <c r="D506" t="inlineStr"/>
@@ -9220,7 +9220,7 @@
         </is>
       </c>
       <c r="B507" t="n">
-        <v>1050</v>
+        <v>650</v>
       </c>
       <c r="C507" t="inlineStr"/>
       <c r="D507" t="inlineStr"/>
@@ -9236,7 +9236,7 @@
         </is>
       </c>
       <c r="B508" t="n">
-        <v>3050</v>
+        <v>2650</v>
       </c>
       <c r="C508" t="inlineStr"/>
       <c r="D508" t="inlineStr"/>
@@ -9268,7 +9268,7 @@
         </is>
       </c>
       <c r="B510" t="n">
-        <v>2050</v>
+        <v>950</v>
       </c>
       <c r="C510" t="inlineStr"/>
       <c r="D510" t="inlineStr"/>
@@ -9284,7 +9284,7 @@
         </is>
       </c>
       <c r="B511" t="n">
-        <v>1900</v>
+        <v>1500</v>
       </c>
       <c r="C511" t="inlineStr"/>
       <c r="D511" t="inlineStr"/>
@@ -9316,7 +9316,7 @@
         </is>
       </c>
       <c r="B513" t="n">
-        <v>1000</v>
+        <v>-650</v>
       </c>
       <c r="C513" t="inlineStr"/>
       <c r="D513" t="inlineStr"/>
@@ -9332,7 +9332,7 @@
         </is>
       </c>
       <c r="B514" t="n">
-        <v>3500</v>
+        <v>2750</v>
       </c>
       <c r="C514" t="inlineStr"/>
       <c r="D514" t="inlineStr"/>
@@ -9364,7 +9364,7 @@
         </is>
       </c>
       <c r="B516" t="n">
-        <v>1600</v>
+        <v>1150</v>
       </c>
       <c r="C516" t="inlineStr"/>
       <c r="D516" t="inlineStr"/>
@@ -9380,7 +9380,7 @@
         </is>
       </c>
       <c r="B517" t="n">
-        <v>3100</v>
+        <v>2850</v>
       </c>
       <c r="C517" t="inlineStr"/>
       <c r="D517" t="inlineStr"/>
@@ -9396,7 +9396,7 @@
         </is>
       </c>
       <c r="B518" t="n">
-        <v>850</v>
+        <v>700</v>
       </c>
       <c r="C518" t="inlineStr"/>
       <c r="D518" t="inlineStr"/>
@@ -9428,7 +9428,7 @@
         </is>
       </c>
       <c r="B520" t="n">
-        <v>900</v>
+        <v>6080</v>
       </c>
       <c r="C520" t="inlineStr"/>
       <c r="D520" t="inlineStr"/>
@@ -9460,7 +9460,7 @@
         </is>
       </c>
       <c r="B522" t="n">
-        <v>3400</v>
+        <v>3300</v>
       </c>
       <c r="C522" t="inlineStr"/>
       <c r="D522" t="inlineStr"/>
@@ -9492,7 +9492,7 @@
         </is>
       </c>
       <c r="B524" t="n">
-        <v>2800</v>
+        <v>1950</v>
       </c>
       <c r="C524" t="inlineStr">
         <is>
@@ -9544,7 +9544,7 @@
         </is>
       </c>
       <c r="B527" t="n">
-        <v>2750</v>
+        <v>1650</v>
       </c>
       <c r="C527" t="inlineStr"/>
       <c r="D527" t="inlineStr"/>
@@ -9622,7 +9622,7 @@
         </is>
       </c>
       <c r="B532" t="n">
-        <v>2950</v>
+        <v>2800</v>
       </c>
       <c r="C532" t="inlineStr"/>
       <c r="D532" t="inlineStr"/>
@@ -9668,7 +9668,7 @@
         </is>
       </c>
       <c r="B535" t="n">
-        <v>1800</v>
+        <v>2700</v>
       </c>
       <c r="C535" t="inlineStr"/>
       <c r="D535" t="inlineStr"/>
@@ -9684,7 +9684,7 @@
         </is>
       </c>
       <c r="B536" t="n">
-        <v>2550</v>
+        <v>2500</v>
       </c>
       <c r="C536" t="inlineStr"/>
       <c r="D536" t="inlineStr"/>
@@ -9700,7 +9700,7 @@
         </is>
       </c>
       <c r="B537" t="n">
-        <v>50000</v>
+        <v>50200</v>
       </c>
       <c r="C537" t="inlineStr"/>
       <c r="D537" t="inlineStr"/>
@@ -9728,7 +9728,7 @@
         </is>
       </c>
       <c r="B539" t="n">
-        <v>41750</v>
+        <v>41150</v>
       </c>
       <c r="C539" t="inlineStr">
         <is>
@@ -9796,7 +9796,7 @@
         </is>
       </c>
       <c r="B542" t="n">
-        <v>12600</v>
+        <v>9450</v>
       </c>
       <c r="C542" t="inlineStr">
         <is>
@@ -9820,7 +9820,7 @@
         </is>
       </c>
       <c r="B543" t="n">
-        <v>7100</v>
+        <v>6100</v>
       </c>
       <c r="C543" t="inlineStr">
         <is>
@@ -9844,7 +9844,7 @@
         </is>
       </c>
       <c r="B544" t="n">
-        <v>-2300</v>
+        <v>-4800</v>
       </c>
       <c r="C544" t="inlineStr">
         <is>
@@ -9892,7 +9892,7 @@
         </is>
       </c>
       <c r="B546" t="n">
-        <v>11800</v>
+        <v>9700</v>
       </c>
       <c r="C546" t="inlineStr">
         <is>
@@ -9916,7 +9916,7 @@
         </is>
       </c>
       <c r="B547" t="n">
-        <v>15900</v>
+        <v>50850</v>
       </c>
       <c r="C547" t="inlineStr">
         <is>
@@ -9976,7 +9976,7 @@
         </is>
       </c>
       <c r="B550" t="n">
-        <v>2000</v>
+        <v>1700</v>
       </c>
       <c r="C550" t="inlineStr">
         <is>
@@ -9996,7 +9996,7 @@
         </is>
       </c>
       <c r="B551" t="n">
-        <v>100</v>
+        <v>-100</v>
       </c>
       <c r="C551" t="inlineStr">
         <is>
@@ -10016,7 +10016,7 @@
         </is>
       </c>
       <c r="B552" t="n">
-        <v>-29000</v>
+        <v>-31000</v>
       </c>
       <c r="C552" t="inlineStr"/>
       <c r="D552" t="inlineStr"/>
@@ -10118,7 +10118,7 @@
         </is>
       </c>
       <c r="B558" t="n">
-        <v>2700</v>
+        <v>2100</v>
       </c>
       <c r="C558" t="inlineStr"/>
       <c r="D558" t="inlineStr"/>
@@ -10174,7 +10174,7 @@
         </is>
       </c>
       <c r="B561" t="n">
-        <v>50</v>
+        <v>-150</v>
       </c>
       <c r="C561" t="inlineStr">
         <is>
@@ -10198,7 +10198,7 @@
         </is>
       </c>
       <c r="B562" t="n">
-        <v>3100</v>
+        <v>1300</v>
       </c>
       <c r="C562" t="inlineStr"/>
       <c r="D562" t="inlineStr"/>
@@ -10214,7 +10214,7 @@
         </is>
       </c>
       <c r="B563" t="n">
-        <v>3450</v>
+        <v>3250</v>
       </c>
       <c r="C563" t="inlineStr">
         <is>
@@ -10234,7 +10234,7 @@
         </is>
       </c>
       <c r="B564" t="n">
-        <v>950</v>
+        <v>850</v>
       </c>
       <c r="C564" t="inlineStr">
         <is>
@@ -10274,7 +10274,7 @@
         </is>
       </c>
       <c r="B566" t="n">
-        <v>5550</v>
+        <v>5200</v>
       </c>
       <c r="C566" t="inlineStr">
         <is>
@@ -10334,7 +10334,7 @@
         </is>
       </c>
       <c r="B569" t="n">
-        <v>2700</v>
+        <v>1450</v>
       </c>
       <c r="C569" t="inlineStr">
         <is>
@@ -10402,7 +10402,7 @@
         </is>
       </c>
       <c r="B572" t="n">
-        <v>8000</v>
+        <v>7500</v>
       </c>
       <c r="C572" t="inlineStr">
         <is>
@@ -10446,7 +10446,7 @@
         </is>
       </c>
       <c r="B574" t="n">
-        <v>6900</v>
+        <v>5900</v>
       </c>
       <c r="C574" t="inlineStr">
         <is>
@@ -10466,7 +10466,7 @@
         </is>
       </c>
       <c r="B575" t="n">
-        <v>2700</v>
+        <v>2600</v>
       </c>
       <c r="C575" t="inlineStr">
         <is>
@@ -10486,7 +10486,7 @@
         </is>
       </c>
       <c r="B576" t="n">
-        <v>2400</v>
+        <v>2250</v>
       </c>
       <c r="C576" t="inlineStr">
         <is>
@@ -10506,7 +10506,7 @@
         </is>
       </c>
       <c r="B577" t="n">
-        <v>900</v>
+        <v>1500</v>
       </c>
       <c r="C577" t="inlineStr">
         <is>
@@ -10550,7 +10550,7 @@
         </is>
       </c>
       <c r="B579" t="n">
-        <v>2100</v>
+        <v>1900</v>
       </c>
       <c r="C579" t="inlineStr"/>
       <c r="D579" t="inlineStr"/>
@@ -10566,7 +10566,7 @@
         </is>
       </c>
       <c r="B580" t="n">
-        <v>600</v>
+        <v>250</v>
       </c>
       <c r="C580" t="inlineStr"/>
       <c r="D580" t="inlineStr"/>
@@ -10582,7 +10582,7 @@
         </is>
       </c>
       <c r="B581" t="n">
-        <v>2900</v>
+        <v>2800</v>
       </c>
       <c r="C581" t="inlineStr"/>
       <c r="D581" t="inlineStr"/>
@@ -10622,7 +10622,7 @@
         </is>
       </c>
       <c r="B583" t="n">
-        <v>800</v>
+        <v>0</v>
       </c>
       <c r="C583" t="inlineStr">
         <is>
@@ -10682,7 +10682,7 @@
         </is>
       </c>
       <c r="B586" t="n">
-        <v>2150</v>
+        <v>1900</v>
       </c>
       <c r="C586" t="inlineStr"/>
       <c r="D586" t="inlineStr"/>
@@ -10698,7 +10698,7 @@
         </is>
       </c>
       <c r="B587" t="n">
-        <v>2300</v>
+        <v>1450</v>
       </c>
       <c r="C587" t="inlineStr"/>
       <c r="D587" t="inlineStr"/>
@@ -10730,7 +10730,7 @@
         </is>
       </c>
       <c r="B589" t="n">
-        <v>800</v>
+        <v>650</v>
       </c>
       <c r="C589" t="inlineStr">
         <is>
@@ -10770,7 +10770,7 @@
         </is>
       </c>
       <c r="B591" t="n">
-        <v>1250</v>
+        <v>950</v>
       </c>
       <c r="C591" t="inlineStr"/>
       <c r="D591" t="inlineStr"/>
@@ -10802,7 +10802,7 @@
         </is>
       </c>
       <c r="B593" t="n">
-        <v>1800</v>
+        <v>1700</v>
       </c>
       <c r="C593" t="inlineStr"/>
       <c r="D593" t="inlineStr"/>
@@ -10818,7 +10818,7 @@
         </is>
       </c>
       <c r="B594" t="n">
-        <v>3600</v>
+        <v>1600</v>
       </c>
       <c r="C594" t="inlineStr"/>
       <c r="D594" t="inlineStr"/>
@@ -10878,7 +10878,7 @@
         </is>
       </c>
       <c r="B597" t="n">
-        <v>2100</v>
+        <v>1800</v>
       </c>
       <c r="C597" t="inlineStr">
         <is>
@@ -10934,7 +10934,7 @@
         </is>
       </c>
       <c r="B599" t="n">
-        <v>3700</v>
+        <v>3850</v>
       </c>
       <c r="C599" t="inlineStr">
         <is>
@@ -10958,7 +10958,7 @@
         </is>
       </c>
       <c r="B600" t="n">
-        <v>1350</v>
+        <v>1150</v>
       </c>
       <c r="C600" t="inlineStr"/>
       <c r="D600" t="inlineStr"/>
@@ -10990,7 +10990,7 @@
         </is>
       </c>
       <c r="B602" t="n">
-        <v>1250</v>
+        <v>1850</v>
       </c>
       <c r="C602" t="inlineStr"/>
       <c r="D602" t="inlineStr"/>
@@ -11006,7 +11006,7 @@
         </is>
       </c>
       <c r="B603" t="n">
-        <v>900</v>
+        <v>500</v>
       </c>
       <c r="C603" t="inlineStr">
         <is>
@@ -11046,7 +11046,7 @@
         </is>
       </c>
       <c r="B605" t="n">
-        <v>800</v>
+        <v>600</v>
       </c>
       <c r="C605" t="inlineStr"/>
       <c r="D605" t="inlineStr"/>
@@ -11078,7 +11078,7 @@
         </is>
       </c>
       <c r="B607" t="n">
-        <v>1300</v>
+        <v>1500</v>
       </c>
       <c r="C607" t="inlineStr"/>
       <c r="D607" t="inlineStr"/>
@@ -11094,7 +11094,7 @@
         </is>
       </c>
       <c r="B608" t="n">
-        <v>1200</v>
+        <v>250</v>
       </c>
       <c r="C608" t="inlineStr"/>
       <c r="D608" t="inlineStr"/>
@@ -11110,7 +11110,7 @@
         </is>
       </c>
       <c r="B609" t="n">
-        <v>2300</v>
+        <v>1700</v>
       </c>
       <c r="C609" t="inlineStr"/>
       <c r="D609" t="inlineStr"/>
@@ -11126,7 +11126,7 @@
         </is>
       </c>
       <c r="B610" t="n">
-        <v>1100</v>
+        <v>850</v>
       </c>
       <c r="C610" t="inlineStr">
         <is>
@@ -11162,7 +11162,7 @@
         </is>
       </c>
       <c r="B612" t="n">
-        <v>1700</v>
+        <v>1400</v>
       </c>
       <c r="C612" t="inlineStr">
         <is>
@@ -11182,7 +11182,7 @@
         </is>
       </c>
       <c r="B613" t="n">
-        <v>4900</v>
+        <v>2800</v>
       </c>
       <c r="C613" t="inlineStr"/>
       <c r="D613" t="inlineStr"/>
@@ -11214,7 +11214,7 @@
         </is>
       </c>
       <c r="B615" t="n">
-        <v>800</v>
+        <v>650</v>
       </c>
       <c r="C615" t="inlineStr"/>
       <c r="D615" t="inlineStr"/>
@@ -11230,7 +11230,7 @@
         </is>
       </c>
       <c r="B616" t="n">
-        <v>450</v>
+        <v>300</v>
       </c>
       <c r="C616" t="inlineStr">
         <is>
@@ -11254,7 +11254,7 @@
         </is>
       </c>
       <c r="B617" t="n">
-        <v>7500</v>
+        <v>7400</v>
       </c>
       <c r="C617" t="inlineStr">
         <is>
@@ -11274,7 +11274,7 @@
         </is>
       </c>
       <c r="B618" t="n">
-        <v>6300</v>
+        <v>6000</v>
       </c>
       <c r="C618" t="inlineStr">
         <is>
@@ -11310,7 +11310,7 @@
         </is>
       </c>
       <c r="B620" t="n">
-        <v>4800</v>
+        <v>4650</v>
       </c>
       <c r="C620" t="inlineStr">
         <is>
@@ -11362,7 +11362,7 @@
         </is>
       </c>
       <c r="B622" t="n">
-        <v>4800</v>
+        <v>4100</v>
       </c>
       <c r="C622" t="inlineStr">
         <is>
@@ -11386,7 +11386,7 @@
         </is>
       </c>
       <c r="B623" t="n">
-        <v>1400</v>
+        <v>1650</v>
       </c>
       <c r="C623" t="inlineStr">
         <is>
@@ -11446,7 +11446,7 @@
         </is>
       </c>
       <c r="B626" t="n">
-        <v>2500</v>
+        <v>2400</v>
       </c>
       <c r="C626" t="inlineStr">
         <is>
@@ -11512,7 +11512,7 @@
         </is>
       </c>
       <c r="B630" t="n">
-        <v>2200</v>
+        <v>1900</v>
       </c>
       <c r="C630" t="inlineStr"/>
       <c r="D630" t="inlineStr"/>
@@ -11528,7 +11528,7 @@
         </is>
       </c>
       <c r="B631" t="n">
-        <v>850</v>
+        <v>4950</v>
       </c>
       <c r="C631" t="inlineStr">
         <is>
@@ -11552,7 +11552,7 @@
         </is>
       </c>
       <c r="B632" t="n">
-        <v>650</v>
+        <v>4200</v>
       </c>
       <c r="C632" t="inlineStr">
         <is>
@@ -11576,7 +11576,7 @@
         </is>
       </c>
       <c r="B633" t="n">
-        <v>519</v>
+        <v>8269</v>
       </c>
       <c r="C633" t="inlineStr">
         <is>
@@ -11624,7 +11624,7 @@
         </is>
       </c>
       <c r="B635" t="n">
-        <v>2100</v>
+        <v>1500</v>
       </c>
       <c r="C635" t="inlineStr">
         <is>
@@ -11672,7 +11672,7 @@
         </is>
       </c>
       <c r="B637" t="n">
-        <v>250</v>
+        <v>150</v>
       </c>
       <c r="C637" t="inlineStr">
         <is>
@@ -11696,7 +11696,7 @@
         </is>
       </c>
       <c r="B638" t="n">
-        <v>1350</v>
+        <v>1150</v>
       </c>
       <c r="C638" t="inlineStr">
         <is>
@@ -11758,7 +11758,7 @@
         </is>
       </c>
       <c r="B641" t="n">
-        <v>5600</v>
+        <v>5500</v>
       </c>
       <c r="C641" t="inlineStr"/>
       <c r="D641" t="inlineStr"/>
@@ -11774,7 +11774,7 @@
         </is>
       </c>
       <c r="B642" t="n">
-        <v>1400</v>
+        <v>1450</v>
       </c>
       <c r="C642" t="inlineStr"/>
       <c r="D642" t="inlineStr"/>

</xml_diff>

<commit_message>
Filter out-of-stock alternates: Only show items with In Stock or Low Stock status as alternatives
</commit_message>
<xml_diff>
--- a/data/master_df.xlsx
+++ b/data/master_df.xlsx
@@ -1988,7 +1988,7 @@
         </is>
       </c>
       <c r="B90" t="n">
-        <v>-18</v>
+        <v>-19</v>
       </c>
       <c r="C90" t="inlineStr"/>
       <c r="D90" t="inlineStr"/>
@@ -2002,7 +2002,7 @@
         </is>
       </c>
       <c r="B91" t="n">
-        <v>-57</v>
+        <v>-59</v>
       </c>
       <c r="C91" t="inlineStr"/>
       <c r="D91" t="inlineStr"/>
@@ -2086,7 +2086,7 @@
         </is>
       </c>
       <c r="B97" t="n">
-        <v>-49</v>
+        <v>-50</v>
       </c>
       <c r="C97" t="inlineStr"/>
       <c r="D97" t="inlineStr"/>
@@ -2142,7 +2142,7 @@
         </is>
       </c>
       <c r="B101" t="n">
-        <v>1750</v>
+        <v>1450</v>
       </c>
       <c r="C101" t="inlineStr"/>
       <c r="D101" t="inlineStr"/>
@@ -2254,7 +2254,7 @@
         </is>
       </c>
       <c r="B108" t="n">
-        <v>2000</v>
+        <v>1900</v>
       </c>
       <c r="C108" t="inlineStr"/>
       <c r="D108" t="inlineStr"/>
@@ -2334,7 +2334,7 @@
         </is>
       </c>
       <c r="B113" t="n">
-        <v>850</v>
+        <v>700</v>
       </c>
       <c r="C113" t="inlineStr"/>
       <c r="D113" t="inlineStr"/>
@@ -3068,7 +3068,7 @@
         </is>
       </c>
       <c r="B158" t="n">
-        <v>3850</v>
+        <v>3650</v>
       </c>
       <c r="C158" t="inlineStr"/>
       <c r="D158" t="inlineStr"/>
@@ -3380,7 +3380,7 @@
         </is>
       </c>
       <c r="B176" t="n">
-        <v>7500</v>
+        <v>7200</v>
       </c>
       <c r="C176" t="inlineStr">
         <is>
@@ -4112,7 +4112,7 @@
         </is>
       </c>
       <c r="B213" t="n">
-        <v>3600</v>
+        <v>3750</v>
       </c>
       <c r="C213" t="inlineStr">
         <is>
@@ -4240,7 +4240,7 @@
         </is>
       </c>
       <c r="B220" t="n">
-        <v>4500</v>
+        <v>4400</v>
       </c>
       <c r="C220" t="inlineStr">
         <is>
@@ -4408,7 +4408,7 @@
         </is>
       </c>
       <c r="B229" t="n">
-        <v>3950</v>
+        <v>3750</v>
       </c>
       <c r="C229" t="inlineStr">
         <is>
@@ -5466,7 +5466,7 @@
         </is>
       </c>
       <c r="B287" t="n">
-        <v>3150</v>
+        <v>2950</v>
       </c>
       <c r="C287" t="inlineStr"/>
       <c r="D287" t="inlineStr"/>
@@ -5530,7 +5530,7 @@
         </is>
       </c>
       <c r="B291" t="n">
-        <v>1450</v>
+        <v>1300</v>
       </c>
       <c r="C291" t="inlineStr"/>
       <c r="D291" t="inlineStr"/>
@@ -5688,7 +5688,7 @@
         </is>
       </c>
       <c r="B300" t="n">
-        <v>1750</v>
+        <v>1600</v>
       </c>
       <c r="C300" t="inlineStr">
         <is>
@@ -5732,7 +5732,7 @@
         </is>
       </c>
       <c r="B302" t="n">
-        <v>1100</v>
+        <v>800</v>
       </c>
       <c r="C302" t="inlineStr">
         <is>
@@ -5948,7 +5948,7 @@
         </is>
       </c>
       <c r="B313" t="n">
-        <v>2600</v>
+        <v>1900</v>
       </c>
       <c r="C313" t="inlineStr">
         <is>
@@ -6052,7 +6052,7 @@
         </is>
       </c>
       <c r="B318" t="n">
-        <v>2900</v>
+        <v>2500</v>
       </c>
       <c r="C318" t="inlineStr"/>
       <c r="D318" t="inlineStr"/>
@@ -6332,7 +6332,7 @@
         </is>
       </c>
       <c r="B333" t="n">
-        <v>-1000</v>
+        <v>-1150</v>
       </c>
       <c r="C333" t="inlineStr"/>
       <c r="D333" t="inlineStr"/>
@@ -6424,7 +6424,7 @@
         </is>
       </c>
       <c r="B338" t="n">
-        <v>2050</v>
+        <v>1850</v>
       </c>
       <c r="C338" t="inlineStr">
         <is>
@@ -6720,7 +6720,7 @@
         </is>
       </c>
       <c r="B354" t="n">
-        <v>1400</v>
+        <v>1300</v>
       </c>
       <c r="C354" t="inlineStr"/>
       <c r="D354" t="inlineStr"/>
@@ -6812,7 +6812,7 @@
         </is>
       </c>
       <c r="B359" t="n">
-        <v>200</v>
+        <v>50</v>
       </c>
       <c r="C359" t="inlineStr"/>
       <c r="D359" t="inlineStr"/>
@@ -7704,7 +7704,7 @@
         </is>
       </c>
       <c r="B411" t="n">
-        <v>1600</v>
+        <v>1300</v>
       </c>
       <c r="C411" t="inlineStr"/>
       <c r="D411" t="inlineStr"/>
@@ -8338,7 +8338,7 @@
         </is>
       </c>
       <c r="B451" t="n">
-        <v>300</v>
+        <v>0</v>
       </c>
       <c r="C451" t="inlineStr"/>
       <c r="D451" t="inlineStr"/>
@@ -8930,7 +8930,7 @@
         </is>
       </c>
       <c r="B489" t="n">
-        <v>6150</v>
+        <v>5800</v>
       </c>
       <c r="C489" t="inlineStr"/>
       <c r="D489" t="inlineStr"/>
@@ -8946,7 +8946,7 @@
         </is>
       </c>
       <c r="B490" t="n">
-        <v>3600</v>
+        <v>3300</v>
       </c>
       <c r="C490" t="inlineStr"/>
       <c r="D490" t="inlineStr"/>
@@ -9136,7 +9136,7 @@
         </is>
       </c>
       <c r="B502" t="n">
-        <v>1950</v>
+        <v>1750</v>
       </c>
       <c r="C502" t="inlineStr">
         <is>
@@ -9156,7 +9156,7 @@
         </is>
       </c>
       <c r="B503" t="n">
-        <v>2200</v>
+        <v>2050</v>
       </c>
       <c r="C503" t="inlineStr"/>
       <c r="D503" t="inlineStr"/>
@@ -9492,7 +9492,7 @@
         </is>
       </c>
       <c r="B524" t="n">
-        <v>1950</v>
+        <v>1750</v>
       </c>
       <c r="C524" t="inlineStr">
         <is>
@@ -9684,7 +9684,7 @@
         </is>
       </c>
       <c r="B536" t="n">
-        <v>2500</v>
+        <v>1500</v>
       </c>
       <c r="C536" t="inlineStr"/>
       <c r="D536" t="inlineStr"/>
@@ -9728,7 +9728,7 @@
         </is>
       </c>
       <c r="B539" t="n">
-        <v>41150</v>
+        <v>40850</v>
       </c>
       <c r="C539" t="inlineStr">
         <is>
@@ -10118,7 +10118,7 @@
         </is>
       </c>
       <c r="B558" t="n">
-        <v>2100</v>
+        <v>1500</v>
       </c>
       <c r="C558" t="inlineStr"/>
       <c r="D558" t="inlineStr"/>
@@ -10446,7 +10446,7 @@
         </is>
       </c>
       <c r="B574" t="n">
-        <v>5900</v>
+        <v>5500</v>
       </c>
       <c r="C574" t="inlineStr">
         <is>
@@ -10818,7 +10818,7 @@
         </is>
       </c>
       <c r="B594" t="n">
-        <v>1600</v>
+        <v>1400</v>
       </c>
       <c r="C594" t="inlineStr"/>
       <c r="D594" t="inlineStr"/>
@@ -10990,7 +10990,7 @@
         </is>
       </c>
       <c r="B602" t="n">
-        <v>1850</v>
+        <v>1650</v>
       </c>
       <c r="C602" t="inlineStr"/>
       <c r="D602" t="inlineStr"/>
@@ -11094,7 +11094,7 @@
         </is>
       </c>
       <c r="B608" t="n">
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="C608" t="inlineStr"/>
       <c r="D608" t="inlineStr"/>
@@ -11446,7 +11446,7 @@
         </is>
       </c>
       <c r="B626" t="n">
-        <v>2400</v>
+        <v>2300</v>
       </c>
       <c r="C626" t="inlineStr">
         <is>
@@ -11552,7 +11552,7 @@
         </is>
       </c>
       <c r="B632" t="n">
-        <v>4200</v>
+        <v>4150</v>
       </c>
       <c r="C632" t="inlineStr">
         <is>
@@ -11624,7 +11624,7 @@
         </is>
       </c>
       <c r="B635" t="n">
-        <v>1500</v>
+        <v>1300</v>
       </c>
       <c r="C635" t="inlineStr">
         <is>
@@ -11758,7 +11758,7 @@
         </is>
       </c>
       <c r="B641" t="n">
-        <v>5500</v>
+        <v>5450</v>
       </c>
       <c r="C641" t="inlineStr"/>
       <c r="D641" t="inlineStr"/>

</xml_diff>